<commit_message>
Mounting pad additions, footswitch and BOM changes
</commit_message>
<xml_diff>
--- a/MainBoard/inspireFly_PQ_mainboard_rev0.1.xlsx
+++ b/MainBoard/inspireFly_PQ_mainboard_rev0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Documents\GitHub\inspireFly-pocketqubeBoards\MainBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68D4FD1-67C2-404F-9F6B-58D07B492128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ED4C46-4F5A-43BD-BB76-32482BACAA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="21795" windowHeight="12975" xr2:uid="{90A7F372-49DC-4743-8A39-617F3F98A630}"/>
+    <workbookView xWindow="705" yWindow="705" windowWidth="16200" windowHeight="9308" xr2:uid="{90A7F372-49DC-4743-8A39-617F3F98A630}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordering Sheet" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>CPF0402B280KE1</t>
   </si>
   <si>
-    <t>RNCF0805BTE250K</t>
-  </si>
-  <si>
     <t>ERA-2ARB622X</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>CPF 0402 280K 0.1% 25PPM 1K RL</t>
   </si>
   <si>
-    <t>RES SMD 250K OHM 0.1% 1/4W 0805</t>
-  </si>
-  <si>
     <t>AOTA-B201210SR47MT</t>
   </si>
   <si>
@@ -650,6 +644,12 @@
   </si>
   <si>
     <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>ERA-2AEB8252X</t>
+  </si>
+  <si>
+    <t>RES SMD 82.5KOHM 0.1% 1/16W 0402</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5925212D-D2B1-4AA1-8E95-17EB777828EB}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1510,7 +1510,7 @@
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1532,10 +1532,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>203</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1545,11 +1545,11 @@
         <v>5</v>
       </c>
       <c r="F20" s="4">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1582,10 +1582,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1607,10 +1607,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
         <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1632,10 +1632,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
         <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1657,10 +1657,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1682,10 +1682,10 @@
         <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1707,10 +1707,10 @@
         <v>10</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1732,10 +1732,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1757,10 +1757,10 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -1782,10 +1782,10 @@
         <v>10</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1807,10 +1807,10 @@
         <v>10</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1832,10 +1832,10 @@
         <v>10</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1857,10 +1857,10 @@
         <v>10</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1882,10 +1882,10 @@
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1907,10 +1907,10 @@
         <v>10</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1932,10 +1932,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1957,10 +1957,10 @@
         <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1982,10 +1982,10 @@
         <v>10</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2007,10 +2007,10 @@
         <v>10</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -2032,10 +2032,10 @@
         <v>10</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -2057,10 +2057,10 @@
         <v>10</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2082,10 +2082,10 @@
         <v>10</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2107,10 +2107,10 @@
         <v>10</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2132,10 +2132,10 @@
         <v>10</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2154,11 +2154,11 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G46" s="2">
         <f>SUM(G2:G44)</f>
-        <v>314.13999999999993</v>
+        <v>314.03999999999991</v>
       </c>
     </row>
   </sheetData>
@@ -2174,30 +2174,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD8EA32-5678-41C9-92DA-56BDDCDB8FAB}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -2205,13 +2205,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
         <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" t="s">
-        <v>116</v>
       </c>
       <c r="G2">
         <v>24</v>
@@ -2222,13 +2222,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -2239,13 +2239,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" t="s">
         <v>119</v>
-      </c>
-      <c r="E4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" t="s">
-        <v>121</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -2256,13 +2256,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2273,13 +2273,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -2290,13 +2290,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -2307,13 +2307,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -2324,13 +2324,13 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -2341,13 +2341,13 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -2358,13 +2358,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G11">
         <v>5</v>
@@ -2375,13 +2375,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -2392,13 +2392,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -2409,13 +2409,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G14">
         <v>3</v>
@@ -2426,13 +2426,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2443,13 +2443,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E16" t="s">
         <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -2460,13 +2460,13 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -2477,13 +2477,13 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2494,13 +2494,13 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -2511,13 +2511,13 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
         <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2528,13 +2528,13 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2545,13 +2545,13 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2562,13 +2562,13 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E23" t="s">
         <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2579,13 +2579,13 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E24">
         <v>120</v>
       </c>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2596,13 +2596,13 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" t="s">
         <v>150</v>
-      </c>
-      <c r="E25" t="s">
-        <v>151</v>
-      </c>
-      <c r="F25" t="s">
-        <v>152</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2613,13 +2613,13 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2630,13 +2630,13 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -2647,13 +2647,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" t="s">
         <v>157</v>
-      </c>
-      <c r="E28" t="s">
-        <v>158</v>
-      </c>
-      <c r="F28" t="s">
-        <v>159</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2664,13 +2664,13 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -2681,13 +2681,13 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -2698,13 +2698,13 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -2715,13 +2715,13 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -2732,13 +2732,13 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2749,13 +2749,13 @@
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -2766,13 +2766,13 @@
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2783,13 +2783,13 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2800,13 +2800,13 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -2817,13 +2817,13 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -2834,13 +2834,13 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G39">
         <v>2</v>
@@ -2851,13 +2851,13 @@
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G40">
         <v>4</v>
@@ -2868,13 +2868,13 @@
         <v>40</v>
       </c>
       <c r="D41" t="s">
+        <v>181</v>
+      </c>
+      <c r="E41" t="s">
+        <v>182</v>
+      </c>
+      <c r="F41" t="s">
         <v>183</v>
-      </c>
-      <c r="E41" t="s">
-        <v>184</v>
-      </c>
-      <c r="F41" t="s">
-        <v>185</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -2885,13 +2885,13 @@
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -2902,13 +2902,13 @@
         <v>42</v>
       </c>
       <c r="D43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" t="s">
+        <v>187</v>
+      </c>
+      <c r="F43" t="s">
         <v>188</v>
-      </c>
-      <c r="E43" t="s">
-        <v>189</v>
-      </c>
-      <c r="F43" t="s">
-        <v>190</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2919,13 +2919,13 @@
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F44" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -2936,13 +2936,13 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2953,13 +2953,13 @@
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2970,13 +2970,13 @@
         <v>46</v>
       </c>
       <c r="D47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E47" t="s">
+        <v>196</v>
+      </c>
+      <c r="F47" t="s">
         <v>197</v>
-      </c>
-      <c r="E47" t="s">
-        <v>198</v>
-      </c>
-      <c r="F47" t="s">
-        <v>199</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2987,13 +2987,13 @@
         <v>47</v>
       </c>
       <c r="D48" t="s">
+        <v>198</v>
+      </c>
+      <c r="E48" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" t="s">
         <v>200</v>
-      </c>
-      <c r="E48" t="s">
-        <v>201</v>
-      </c>
-      <c r="F48" t="s">
-        <v>202</v>
       </c>
       <c r="G48">
         <v>1</v>

</xml_diff>

<commit_message>
Final Board Order Changes for Mainboard
</commit_message>
<xml_diff>
--- a/MainBoard/inspireFly_PQ_mainboard_rev0.1.xlsx
+++ b/MainBoard/inspireFly_PQ_mainboard_rev0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Documents\GitHub\inspireFly-pocketqubeBoards\MainBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ED4C46-4F5A-43BD-BB76-32482BACAA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2559A68-0FDD-4BC6-ADC1-92390E168A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="705" windowWidth="16200" windowHeight="9308" xr2:uid="{90A7F372-49DC-4743-8A39-617F3F98A630}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{90A7F372-49DC-4743-8A39-617F3F98A630}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordering Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="210">
   <si>
     <t>Part Number</t>
   </si>
@@ -121,9 +121,6 @@
     <t>CAP CER 0.47UF 10V X7R 0402</t>
   </si>
   <si>
-    <t>100K</t>
-  </si>
-  <si>
     <t>5m</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>280k</t>
   </si>
   <si>
-    <t>250k</t>
-  </si>
-  <si>
     <t>6.2k</t>
   </si>
   <si>
@@ -253,12 +247,6 @@
     <t>DIODE SCHOTTKY 20V 2A DO219AD</t>
   </si>
   <si>
-    <t>XZMDK68W-2</t>
-  </si>
-  <si>
-    <t>LED RED CLEAR CHIP SMD</t>
-  </si>
-  <si>
     <t>INA185A4IDRLR</t>
   </si>
   <si>
@@ -442,9 +430,6 @@
     <t>R_0402_1005Metric</t>
   </si>
   <si>
-    <t>R4, R22, R32, R34</t>
-  </si>
-  <si>
     <t>R21, R29, R31, R33</t>
   </si>
   <si>
@@ -454,12 +439,6 @@
     <t>R1, R2, R5</t>
   </si>
   <si>
-    <t>R10, R24, R26</t>
-  </si>
-  <si>
-    <t>R3, R14</t>
-  </si>
-  <si>
     <t>R12, R19</t>
   </si>
   <si>
@@ -469,9 +448,6 @@
     <t>R11</t>
   </si>
   <si>
-    <t>R15</t>
-  </si>
-  <si>
     <t>R16</t>
   </si>
   <si>
@@ -508,21 +484,12 @@
     <t>D2</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>LED_0402_1005Metric</t>
-  </si>
-  <si>
     <t>U1, U11</t>
   </si>
   <si>
     <t>SOT_INA185_TEX</t>
   </si>
   <si>
-    <t>U10, U12</t>
-  </si>
-  <si>
     <t>SOT_V-T1-GE3_VIS-M</t>
   </si>
   <si>
@@ -619,37 +586,88 @@
     <t>USB4110-GF-A_GCT</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>HARWIN_M55-7104042R</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>PinHeader_2x02_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Conn_01x02_Pin</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
     <t>ERA-2AEB8252X</t>
   </si>
   <si>
     <t>RES SMD 82.5KOHM 0.1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>R3, R15</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>82.5k</t>
+  </si>
+  <si>
+    <t>LTST-S270KRKT</t>
+  </si>
+  <si>
+    <t>LED_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>FTSW EN</t>
+  </si>
+  <si>
+    <t>SmallJumper</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>NRBG104F3435B2F</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR CHIP SMD R/A</t>
+  </si>
+  <si>
+    <t>NTC 10K 3435K BETA 25/85 1%</t>
+  </si>
+  <si>
+    <t>FTSH-107-01-L-DV-K-A</t>
+  </si>
+  <si>
+    <t>BH123A</t>
+  </si>
+  <si>
+    <t>BATTERY HOLDER CR123A PC PIN</t>
+  </si>
+  <si>
+    <t>R4, R6, R22, R32, R34, R35</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>R7, R10, R24, R26</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>Heater</t>
+  </si>
+  <si>
+    <t>HeaterConnection</t>
+  </si>
+  <si>
+    <t>U2, U10, U12</t>
+  </si>
+  <si>
+    <t>BT1, BT2</t>
+  </si>
+  <si>
+    <t>BAT_BH123A</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>SAMTEC_FTSH-107-01-L-DV-K-A</t>
   </si>
 </sst>
 </file>
@@ -1037,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5925212D-D2B1-4AA1-8E95-17EB777828EB}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1123,7 +1141,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G44" si="0" xml:space="preserve"> E3 *F3</f>
+        <f t="shared" ref="G3:G47" si="0" xml:space="preserve"> E3 *F3</f>
         <v>0.15</v>
       </c>
     </row>
@@ -1307,10 +1325,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1332,24 +1350,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <f xml:space="preserve"> D12 *Constants!$C$1</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>1.42</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -1357,10 +1375,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -1382,10 +1400,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -1407,24 +1425,24 @@
         <v>10</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <f xml:space="preserve"> D15 *Constants!$C$1</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F15" s="4">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>1.23</v>
+        <v>1.6400000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -1432,10 +1450,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1457,10 +1475,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1482,10 +1500,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1507,10 +1525,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1532,10 +1550,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1557,10 +1575,10 @@
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
         <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1582,10 +1600,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
         <v>57</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1607,10 +1625,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1632,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1657,10 +1675,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1682,10 +1700,10 @@
         <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1707,10 +1725,10 @@
         <v>10</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1732,10 +1750,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>71</v>
+        <v>187</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>194</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1745,11 +1763,11 @@
         <v>5</v>
       </c>
       <c r="F28" s="4">
-        <v>0.22</v>
+        <v>0.12</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
@@ -1757,10 +1775,10 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -1782,24 +1800,24 @@
         <v>10</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <f xml:space="preserve"> D30 *Constants!$C$1</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F30" s="4">
         <v>0.70699999999999996</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>7.0699999999999994</v>
+        <v>10.604999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -1807,10 +1825,10 @@
         <v>10</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1832,10 +1850,10 @@
         <v>10</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1857,10 +1875,10 @@
         <v>10</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1882,10 +1900,10 @@
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1907,10 +1925,10 @@
         <v>10</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1932,10 +1950,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1957,10 +1975,10 @@
         <v>10</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1982,10 +2000,10 @@
         <v>10</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2007,10 +2025,10 @@
         <v>10</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -2032,10 +2050,10 @@
         <v>10</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -2057,10 +2075,10 @@
         <v>10</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2082,10 +2100,10 @@
         <v>10</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2107,10 +2125,10 @@
         <v>10</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2132,10 +2150,10 @@
         <v>10</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2152,13 +2170,88 @@
         <v>12.3</v>
       </c>
     </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" t="s">
+        <v>195</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f xml:space="preserve"> D45 *Constants!$C$1</f>
+        <v>5</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>10</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C46" t="s">
+        <v>196</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <f xml:space="preserve"> D46 *Constants!$C$1</f>
+        <v>5</v>
+      </c>
+      <c r="F46" s="4">
+        <v>3.21</v>
       </c>
       <c r="G46" s="2">
-        <f>SUM(G2:G44)</f>
-        <v>314.03999999999991</v>
+        <f t="shared" si="0"/>
+        <v>16.05</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C47" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <f xml:space="preserve"> D47 *Constants!$C$1</f>
+        <v>10</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1.101</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="0"/>
+        <v>11.01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="G48" s="2">
+        <f>SUM(G2:G47)</f>
+        <v>348.35499999999996</v>
       </c>
     </row>
   </sheetData>
@@ -2172,32 +2265,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD8EA32-5678-41C9-92DA-56BDDCDB8FAB}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>107</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -2205,13 +2298,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G2">
         <v>24</v>
@@ -2222,13 +2315,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -2239,13 +2332,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -2256,13 +2349,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2273,13 +2366,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -2290,13 +2383,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -2307,13 +2400,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -2324,13 +2417,13 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -2341,13 +2434,13 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -2358,16 +2451,16 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
+        <v>199</v>
+      </c>
+      <c r="E11" t="s">
+        <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -2375,16 +2468,16 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
+        <v>128</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -2392,13 +2485,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -2409,16 +2502,16 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -2426,13 +2519,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2443,13 +2536,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -2460,13 +2553,13 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -2477,13 +2570,13 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2494,13 +2587,13 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>203</v>
       </c>
       <c r="F19" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -2511,13 +2604,13 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>201</v>
+        <v>129</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2528,13 +2621,13 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>186</v>
       </c>
       <c r="F21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2545,13 +2638,13 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2562,13 +2655,13 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2579,13 +2672,13 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
-      </c>
-      <c r="E24">
-        <v>120</v>
+        <v>138</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2596,13 +2689,13 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E25" t="s">
-        <v>149</v>
+        <v>139</v>
+      </c>
+      <c r="E25">
+        <v>120</v>
       </c>
       <c r="F25" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2613,13 +2706,13 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -2630,13 +2723,13 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="F27" t="s">
-        <v>154</v>
+        <v>65</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -2647,13 +2740,13 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E28" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="F28" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2664,16 +2757,16 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>187</v>
       </c>
       <c r="F29" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -2681,16 +2774,16 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -2698,16 +2791,16 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E31" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
@@ -2715,13 +2808,13 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F32" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -2732,13 +2825,13 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -2749,13 +2842,13 @@
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>77</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -2766,13 +2859,13 @@
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2783,13 +2876,13 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F36" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -2800,13 +2893,13 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -2817,13 +2910,13 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="E38" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
       <c r="F38" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -2834,16 +2927,16 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="F39" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
@@ -2851,16 +2944,16 @@
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="F40" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="G40">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
@@ -2868,16 +2961,16 @@
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="E41" t="s">
-        <v>182</v>
+        <v>91</v>
       </c>
       <c r="F41" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
@@ -2885,16 +2978,16 @@
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="F42" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
@@ -2902,13 +2995,13 @@
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="E43" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="F43" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2925,7 +3018,7 @@
         <v>190</v>
       </c>
       <c r="F44" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -2936,13 +3029,13 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F45" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2953,13 +3046,13 @@
         <v>45</v>
       </c>
       <c r="D46" t="s">
+        <v>192</v>
+      </c>
+      <c r="E46" t="s">
         <v>193</v>
       </c>
-      <c r="E46" t="s">
-        <v>103</v>
-      </c>
       <c r="F46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2970,13 +3063,13 @@
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="E47" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="F47" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2987,15 +3080,49 @@
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="E48" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="F48" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>208</v>
+      </c>
+      <c r="E49" t="s">
+        <v>196</v>
+      </c>
+      <c r="F49" t="s">
+        <v>209</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>180</v>
+      </c>
+      <c r="E50" t="s">
+        <v>97</v>
+      </c>
+      <c r="F50" t="s">
+        <v>181</v>
+      </c>
+      <c r="G50">
         <v>1</v>
       </c>
     </row>

</xml_diff>